<commit_message>
Updated library: cPickle (python2) -> pickle (python3) Updated print command syntax: print abc -> print (abc) FFR_river_network file has a field named ERO_YLD_TON, however, during filtering of the database file name of several fields were shortened. One of them is this, which changed to ERO_YLD_TO
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Projects\FFR\FRA\scr\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\GitHub\Free-Flowing-Rivers\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06E191C-AA59-4246-A9D9-2000A661B23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2055" tabRatio="716" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="716" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="33" r:id="rId1"/>
@@ -17,17 +18,29 @@
     <sheet name="SCE_100" sheetId="27" r:id="rId3"/>
     <sheet name="Description of variables" sheetId="36" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="213">
   <si>
     <t>URB</t>
   </si>
@@ -641,25 +654,37 @@
     <t>NO</t>
   </si>
   <si>
-    <t>C:\\FFR\output\</t>
-  </si>
-  <si>
-    <t>C:\\FFR\data.gdb\hydrolakes</t>
-  </si>
-  <si>
-    <t>C:\\FFR\data.gdb\streams</t>
-  </si>
-  <si>
     <t>C:\\FFR\data.gdb\bm_rivers</t>
   </si>
   <si>
-    <t>C:\\FFR\data.gdb\barriers</t>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>D:\RiverATLAS\Global_Dam_Watch_GDW\GDW_filtered\GDW_reservoirs_filtered.shp</t>
+  </si>
+  <si>
+    <t>D:\RiverATLAS\Global_Dam_Watch_GDW\GDW_filtered\GDW_barriers_filtered.shp</t>
+  </si>
+  <si>
+    <t>D:\Peninsular India\Output</t>
+  </si>
+  <si>
+    <t>DOF_try1</t>
+  </si>
+  <si>
+    <t>DOR_try1</t>
+  </si>
+  <si>
+    <t>SED_try1</t>
+  </si>
+  <si>
+    <t>D:\RiverATLAS\Free_Flowing_Rivers\Mapping the worlds free-flowing rivers_Data_Geodatabase\Mapping the worlds free-flowing rivers_Data_Geodatabase\FFR_river_peninsular.gdb\FFR_river_peninsular</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -829,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -848,7 +873,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -856,11 +881,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -985,75 +1006,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1380,6 +1332,75 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1394,15 +1415,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table735" displayName="Table735" ref="A1:D17" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:D17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table735" displayName="Table735" ref="A1:D17" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:D17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="5" name="Category" dataDxfId="28"/>
-    <tableColumn id="3" name="Key" dataDxfId="27">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Key" dataDxfId="22">
       <calculatedColumnFormula>Table8[[#This Row],[Variable name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Value" dataDxfId="26"/>
-    <tableColumn id="2" name="Description" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="20">
       <calculatedColumnFormula>Table8[[#This Row],[Short description]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1411,38 +1432,38 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table273151618" displayName="Table273151618" ref="A1:R123" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table273151618" displayName="Table273151618" ref="A1:R123" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="18">
-    <tableColumn id="1" name="scenario_name" dataDxfId="22"/>
-    <tableColumn id="2" name="indicator_1" dataDxfId="21"/>
-    <tableColumn id="3" name="indicator_2" dataDxfId="20"/>
-    <tableColumn id="16" name="indicator_3" dataDxfId="19"/>
-    <tableColumn id="4" name="indicator_4" dataDxfId="18"/>
-    <tableColumn id="5" name="indicator_5" dataDxfId="17"/>
-    <tableColumn id="6" name="indicator_6" dataDxfId="16"/>
-    <tableColumn id="7" name="weight_1" dataDxfId="15"/>
-    <tableColumn id="8" name="weight_2" dataDxfId="14"/>
-    <tableColumn id="17" name="weight_3" dataDxfId="13"/>
-    <tableColumn id="9" name="weight_4" dataDxfId="12"/>
-    <tableColumn id="10" name="weight_5" dataDxfId="11"/>
-    <tableColumn id="11" name="weight_6" dataDxfId="10"/>
-    <tableColumn id="12" name="csi_thresh" dataDxfId="9"/>
-    <tableColumn id="13" name="fld_damp" dataDxfId="8"/>
-    <tableColumn id="15" name="filter_thresh" dataDxfId="7"/>
-    <tableColumn id="18" name="to_process" dataDxfId="6"/>
-    <tableColumn id="14" name="to_export" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="scenario_name" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="indicator_1" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="indicator_2" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="indicator_3" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="indicator_4" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="indicator_5" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="indicator_6" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="weight_1" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="weight_2" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="weight_3" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="weight_4" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="weight_5" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="weight_6" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="csi_thresh" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="fld_damp" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="filter_thresh" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="to_process" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="to_export" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:C17" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A1:C17" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:C17" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="3">
-    <tableColumn id="4" name="Context" dataDxfId="2"/>
-    <tableColumn id="1" name="Variable name" dataDxfId="1"/>
-    <tableColumn id="2" name="Short description" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Context" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable name" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Short description" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1710,11 +1731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1744,7 @@
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
@@ -1735,7 +1756,7 @@
       <c r="A2" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>191</v>
       </c>
     </row>
@@ -1743,26 +1764,26 @@
       <c r="A3" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>203</v>
+      <c r="B5" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>203</v>
       </c>
     </row>
@@ -1770,7 +1791,7 @@
       <c r="A7" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>203</v>
       </c>
     </row>
@@ -1778,16 +1799,16 @@
       <c r="A8" t="s">
         <v>173</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>31</v>
+      <c r="B8" s="12" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Only use YES or NO" promptTitle="Boolean field" prompt="Please use the dropdown field to enter &quot;YES&quot; or &quot;NO&quot;" sqref="B5:B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Only use YES or NO" promptTitle="Boolean field" prompt="Please use the dropdown field to enter &quot;YES&quot; or &quot;NO&quot;" sqref="B5:B8" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Sheets</formula1>
     </dataValidation>
   </dataValidations>
@@ -1797,310 +1818,310 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36" style="19" customWidth="1"/>
-    <col min="3" max="3" width="141.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="110.7109375" style="39" customWidth="1"/>
-    <col min="5" max="16384" width="60.140625" style="18"/>
+    <col min="1" max="1" width="25.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="17" customWidth="1"/>
+    <col min="3" max="3" width="141.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="110.7109375" style="37" customWidth="1"/>
+    <col min="5" max="16384" width="60.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="23" t="str">
+      <c r="B2" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>dams_fc</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="25" t="str">
+      <c r="C2" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Path to the barrier feature class</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="23" t="str">
+      <c r="B3" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>bench_fc</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="D3" s="25" t="str">
+      <c r="C3" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Path to benchmark feature class</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="23" t="str">
+      <c r="B4" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>streams_fc</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="D4" s="25" t="str">
+      <c r="C4" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Path to the streams feature class</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="23" t="str">
+      <c r="B5" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>lakes_fc</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="25" t="str">
+      <c r="C5" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Path to hydrolakes feature class</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="23" t="str">
+      <c r="B6" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>output_folder</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="25" t="str">
+      <c r="C6" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Output folder for results. Typically in folder "/output" under base directory</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B7" s="28" t="str">
+      <c r="B7" s="26" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>barrier_inc_field</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="29" t="str">
+      <c r="D7" s="27" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Field in the dams/barriers database (dams_fc) that determines which dams are included in the assessment. Applies to DOR / DOF / SED calculations. A value of 0 or 1 indicates to use or not to use the barrier, respectively.</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="28" t="str">
+      <c r="B8" s="26" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>update_mode</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="D8" s="29" t="str">
+      <c r="D8" s="27" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Indicates if DOR, DOF, and SED calculations are written back into the streams feature class after recalculation. Yes or no</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="28" t="str">
+      <c r="B9" s="26" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>min_length</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="26">
         <v>500</v>
       </c>
-      <c r="D9" s="29" t="str">
+      <c r="D9" s="27" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>defines the minimum length at which rivers are included in certain output statistics, e.g. in list of free-flowing rivers or list of good connectivity segments. At global scale it is 500 km.</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="31" t="str">
+      <c r="B10" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>dof_field</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="32" t="str">
+      <c r="C10" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Field to use for storing DOF values</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="31" t="str">
+      <c r="B11" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>drf_upstream</v>
       </c>
-      <c r="C11" s="31">
-        <v>5</v>
-      </c>
-      <c r="D11" s="32" t="str">
+      <c r="C11" s="29">
+        <v>5</v>
+      </c>
+      <c r="D11" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Discharge range factor (drf) used in DOF calculations for upstream direction. Must be larger or equal than 1. A drf of 1 signifies that there is no effect upstream</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="31" t="str">
+      <c r="B12" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>drf_downstream</v>
       </c>
-      <c r="C12" s="31">
-        <v>5</v>
-      </c>
-      <c r="D12" s="32" t="str">
+      <c r="C12" s="29">
+        <v>5</v>
+      </c>
+      <c r="D12" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Discharge range factor (drf) used in DOF calculations for downstream direction. Must be larger or equal than 1. A drf of 1 signifies that there is no effect downstream</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="31" t="str">
+      <c r="B13" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>use_dam_level_df</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="32" t="str">
+      <c r="D13" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>If true, the algorithm uses the fields "DFU" (Discharge factor upstream) and "DFD" (Discharge Factor downstream) to calculate dam-specific DOF results and ignores "drf" settings above</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="B14" s="31" t="str">
+      <c r="B14" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>dof_mode</v>
       </c>
-      <c r="C14" s="31">
-        <v>1</v>
-      </c>
-      <c r="D14" s="32" t="str">
+      <c r="C14" s="29">
+        <v>1</v>
+      </c>
+      <c r="D14" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>DOF decay function type</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B15" s="34" t="str">
+      <c r="B15" s="32" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>dor_field</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="35" t="str">
+      <c r="C15" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" s="33" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Field to use for storing DOR values</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
+    <row r="16" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B16" s="34" t="str">
+      <c r="B16" s="32" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>svol_field</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D16" s="35" t="str">
+      <c r="D16" s="33" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Source field for reservoir storage volume</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="35" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>sed_field</v>
       </c>
-      <c r="C17" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="38" t="str">
+      <c r="C17" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" s="36" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
         <v>Field to use for storing SED values</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2112,12 +2133,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R123"/>
+  <dimension ref="A1:Z123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK9" sqref="AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2157,7 @@
     <col min="19" max="16384" width="5.28515625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="4" customFormat="1" ht="105.75" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -2192,7 +2213,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>52</v>
       </c>
@@ -2248,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>53</v>
       </c>
@@ -2303,8 +2324,11 @@
       <c r="R3" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="Z3" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -2360,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -2416,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>56</v>
       </c>
@@ -2472,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -2528,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
@@ -2584,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>59</v>
       </c>
@@ -2640,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>60</v>
       </c>
@@ -2696,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -2752,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>62</v>
       </c>
@@ -2808,7 +2832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -2864,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -2920,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>65</v>
       </c>
@@ -2976,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>66</v>
       </c>
@@ -9025,8 +9049,110 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P103:P113">
-    <cfRule type="colorScale" priority="49">
+  <conditionalFormatting sqref="H2:M20 H22:M42">
+    <cfRule type="colorScale" priority="296">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="303">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:M20 H22:M101">
+    <cfRule type="colorScale" priority="373">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:M101">
+    <cfRule type="colorScale" priority="377">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21:M21">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H102:M123">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N20 N22:N42 N102:N123">
+    <cfRule type="colorScale" priority="370">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9037,8 +9163,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N102">
-    <cfRule type="colorScale" priority="37">
+  <conditionalFormatting sqref="N2:N20 N22:N42 N103:N123">
+    <cfRule type="colorScale" priority="365">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N20 N22:N42">
+    <cfRule type="colorScale" priority="301">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9049,8 +9187,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P102">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="N2:N20 N22:N123">
+    <cfRule type="colorScale" priority="375">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9061,8 +9199,72 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P102">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="N2:N123">
+    <cfRule type="colorScale" priority="378">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N21">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N43:N101">
+    <cfRule type="colorScale" priority="228">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="226">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9075,6 +9277,86 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="N102">
     <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N103:N113 N115 N117 N119 N121 N123">
+    <cfRule type="colorScale" priority="358">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N116:N123 N114">
+    <cfRule type="colorScale" priority="353">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P20 P22:P42 P103:P123">
+    <cfRule type="colorScale" priority="360">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P20 P22:P42">
+    <cfRule type="colorScale" priority="294">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P21">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9097,8 +9379,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N43:N101">
-    <cfRule type="colorScale" priority="226">
+  <conditionalFormatting sqref="P102">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9109,212 +9401,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N43:N101">
-    <cfRule type="colorScale" priority="228">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P21">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P21">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21:M21">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21:M21">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21:M21">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P20 P22:P42">
-    <cfRule type="colorScale" priority="294">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M20 H22:M42">
-    <cfRule type="colorScale" priority="296">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N20 N22:N42">
-    <cfRule type="colorScale" priority="301">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M20 H22:M42">
-    <cfRule type="colorScale" priority="303">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N116:N123 N114">
-    <cfRule type="colorScale" priority="353">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N103:N113 N115 N117 N119 N121 N123">
-    <cfRule type="colorScale" priority="358">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P20 P22:P42 P103:P123">
-    <cfRule type="colorScale" priority="360">
+  <conditionalFormatting sqref="P103:P113">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9337,20 +9425,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N20 N22:N42 N103:N123">
-    <cfRule type="colorScale" priority="365">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q123">
-    <cfRule type="colorScale" priority="369">
+  <conditionalFormatting sqref="P2:Q123">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9361,80 +9437,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N20 N22:N42 N102:N123">
-    <cfRule type="colorScale" priority="370">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M20 H22:M101">
-    <cfRule type="colorScale" priority="373">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N20 N22:N123">
-    <cfRule type="colorScale" priority="375">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M101">
-    <cfRule type="colorScale" priority="377">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N123">
-    <cfRule type="colorScale" priority="378">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H102:M123">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:Q123">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="Q2:Q123">
+    <cfRule type="colorScale" priority="369">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9454,205 +9458,205 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.28515625" style="40" customWidth="1"/>
-    <col min="4" max="16384" width="44" style="16"/>
+    <col min="1" max="1" width="18.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="78.28515625" style="38" customWidth="1"/>
+    <col min="4" max="16384" width="44" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="44" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="44" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="44" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="44" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="44" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="47" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="47" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="47" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="47" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="47" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="B15" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="52" t="s">
+      <c r="B15" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="50" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="50" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="52" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="53" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made some minor changes Replaced cPickle with pickle in some files Updated file format from .xls to .xlsx in some files
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\GitHub\Free-Flowing-Rivers\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06E191C-AA59-4246-A9D9-2000A661B23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD9BAB-98F3-4100-9F9E-964A62CB7479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="716" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Description of variables" sheetId="36" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -123,9 +122,6 @@
     <t>bench_fc</t>
   </si>
   <si>
-    <t>INC1</t>
-  </si>
-  <si>
     <t>use_dam_level_df</t>
   </si>
   <si>
@@ -519,9 +515,6 @@
     <t>lakes_fc</t>
   </si>
   <si>
-    <t>STOR_MCM</t>
-  </si>
-  <si>
     <t>sed_field</t>
   </si>
   <si>
@@ -679,6 +672,12 @@
   </si>
   <si>
     <t>D:\RiverATLAS\Free_Flowing_Rivers\Mapping the worlds free-flowing rivers_Data_Geodatabase\Mapping the worlds free-flowing rivers_Data_Geodatabase\FFR_river_peninsular.gdb\FFR_river_peninsular</t>
+  </si>
+  <si>
+    <t>CAP_MCM</t>
+  </si>
+  <si>
+    <t>INCLUDE</t>
   </si>
 </sst>
 </file>
@@ -1008,6 +1007,75 @@
   <dxfs count="31">
     <dxf>
       <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1332,75 +1400,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1415,15 +1414,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table735" displayName="Table735" ref="A1:D17" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table735" displayName="Table735" ref="A1:D17" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:D17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Key" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Key" dataDxfId="27">
       <calculatedColumnFormula>Table8[[#This Row],[Variable name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="25">
       <calculatedColumnFormula>Table8[[#This Row],[Short description]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1432,38 +1431,38 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table273151618" displayName="Table273151618" ref="A1:R123" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table273151618" displayName="Table273151618" ref="A1:R123" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="scenario_name" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="indicator_1" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="indicator_2" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="indicator_3" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="indicator_4" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="indicator_5" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="indicator_6" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="weight_1" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="weight_2" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="weight_3" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="weight_4" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="weight_5" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="weight_6" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="csi_thresh" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="fld_damp" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="filter_thresh" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="to_process" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="to_export" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="scenario_name" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="indicator_1" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="indicator_2" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="indicator_3" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="indicator_4" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="indicator_5" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="indicator_6" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="weight_1" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="weight_2" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="weight_3" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="weight_4" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="weight_5" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="weight_6" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="csi_thresh" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="fld_damp" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="filter_thresh" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="to_process" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="to_export" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A1:C17" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A1:C17" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C17" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="3">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Context" dataDxfId="28"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable name" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Short description" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Context" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Short description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1754,18 +1753,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1773,34 +1772,34 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1823,7 +1822,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1837,7 +1836,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>8</v>
@@ -1846,19 +1845,19 @@
         <v>7</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>dams_fc</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D2" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1867,14 +1866,14 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>bench_fc</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D3" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1883,14 +1882,14 @@
     </row>
     <row r="4" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B4" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>streams_fc</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D4" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1899,14 +1898,14 @@
     </row>
     <row r="5" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>lakes_fc</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D5" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1921,14 +1920,14 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="21" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>output_folder</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D6" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1937,14 +1936,14 @@
     </row>
     <row r="7" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B7" s="26" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>barrier_inc_field</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>27</v>
+        <v>212</v>
       </c>
       <c r="D7" s="27" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1953,14 +1952,14 @@
     </row>
     <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="26" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>update_mode</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D8" s="27" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1969,7 +1968,7 @@
     </row>
     <row r="9" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B9" s="26" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
@@ -1985,14 +1984,14 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B10" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>dof_field</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D10" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2001,7 +2000,7 @@
     </row>
     <row r="11" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B11" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
@@ -2017,7 +2016,7 @@
     </row>
     <row r="12" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B12" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
@@ -2033,14 +2032,14 @@
     </row>
     <row r="13" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B13" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>use_dam_level_df</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D13" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2049,7 +2048,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B14" s="29" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
@@ -2065,14 +2064,14 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B15" s="32" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>dor_field</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D15" s="33" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2081,14 +2080,14 @@
     </row>
     <row r="16" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16" s="32" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>svol_field</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>159</v>
+        <v>211</v>
       </c>
       <c r="D16" s="33" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2103,14 +2102,14 @@
     </row>
     <row r="17" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B17" s="35" t="str">
         <f>Table8[[#This Row],[Variable name]]</f>
         <v>sed_field</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D17" s="36" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2177,7 +2176,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2195,7 +2194,7 @@
         <v>22</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>9</v>
@@ -2207,24 +2206,24 @@
         <v>11</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>2</v>
@@ -2271,16 +2270,16 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>2</v>
@@ -2325,21 +2324,21 @@
         <v>0</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>2</v>
@@ -2386,16 +2385,16 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>2</v>
@@ -2442,16 +2441,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>2</v>
@@ -2498,16 +2497,16 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>2</v>
@@ -2554,16 +2553,16 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>2</v>
@@ -2610,16 +2609,16 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>2</v>
@@ -2666,16 +2665,16 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>2</v>
@@ -2722,16 +2721,16 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>2</v>
@@ -2778,16 +2777,16 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>2</v>
@@ -2834,16 +2833,16 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>2</v>
@@ -2890,16 +2889,16 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>2</v>
@@ -2946,16 +2945,16 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>2</v>
@@ -3002,16 +3001,16 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>2</v>
@@ -3058,16 +3057,16 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>2</v>
@@ -3114,16 +3113,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>2</v>
@@ -3170,16 +3169,16 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>2</v>
@@ -3226,16 +3225,16 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>2</v>
@@ -3282,16 +3281,16 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>2</v>
@@ -3338,16 +3337,16 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>2</v>
@@ -3394,16 +3393,16 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>2</v>
@@ -3450,16 +3449,16 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>2</v>
@@ -3506,16 +3505,16 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>2</v>
@@ -3562,16 +3561,16 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>2</v>
@@ -3618,16 +3617,16 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>2</v>
@@ -3674,16 +3673,16 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>2</v>
@@ -3730,16 +3729,16 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>2</v>
@@ -3786,16 +3785,16 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>2</v>
@@ -3842,16 +3841,16 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>2</v>
@@ -3898,16 +3897,16 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>2</v>
@@ -3954,16 +3953,16 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>2</v>
@@ -4010,16 +4009,16 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>2</v>
@@ -4066,16 +4065,16 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>2</v>
@@ -4122,16 +4121,16 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>2</v>
@@ -4178,16 +4177,16 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>2</v>
@@ -4234,16 +4233,16 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>2</v>
@@ -4290,16 +4289,16 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>2</v>
@@ -4346,16 +4345,16 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>2</v>
@@ -4402,16 +4401,16 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>2</v>
@@ -4458,16 +4457,16 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>2</v>
@@ -4514,16 +4513,16 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>2</v>
@@ -4570,16 +4569,16 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>2</v>
@@ -4626,16 +4625,16 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>2</v>
@@ -4682,16 +4681,16 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>2</v>
@@ -4738,16 +4737,16 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>2</v>
@@ -4794,16 +4793,16 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>2</v>
@@ -4850,16 +4849,16 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>2</v>
@@ -4906,16 +4905,16 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>2</v>
@@ -4962,16 +4961,16 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>2</v>
@@ -5018,16 +5017,16 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>2</v>
@@ -5074,16 +5073,16 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>2</v>
@@ -5130,16 +5129,16 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>2</v>
@@ -5186,16 +5185,16 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>2</v>
@@ -5242,16 +5241,16 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>2</v>
@@ -5298,16 +5297,16 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>2</v>
@@ -5354,16 +5353,16 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>2</v>
@@ -5410,16 +5409,16 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>2</v>
@@ -5466,16 +5465,16 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>2</v>
@@ -5522,16 +5521,16 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>2</v>
@@ -5578,16 +5577,16 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>2</v>
@@ -5634,16 +5633,16 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>2</v>
@@ -5690,16 +5689,16 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>2</v>
@@ -5746,16 +5745,16 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>2</v>
@@ -5802,16 +5801,16 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>2</v>
@@ -5858,16 +5857,16 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>2</v>
@@ -5914,16 +5913,16 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>2</v>
@@ -5970,16 +5969,16 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>2</v>
@@ -6026,16 +6025,16 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>2</v>
@@ -6082,16 +6081,16 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>2</v>
@@ -6138,16 +6137,16 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>2</v>
@@ -6194,16 +6193,16 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>2</v>
@@ -6250,16 +6249,16 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>2</v>
@@ -6306,16 +6305,16 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>2</v>
@@ -6362,16 +6361,16 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>2</v>
@@ -6418,16 +6417,16 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>2</v>
@@ -6474,16 +6473,16 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>2</v>
@@ -6530,16 +6529,16 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>2</v>
@@ -6586,16 +6585,16 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>2</v>
@@ -6642,16 +6641,16 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>2</v>
@@ -6698,16 +6697,16 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>2</v>
@@ -6754,16 +6753,16 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>2</v>
@@ -6810,16 +6809,16 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>2</v>
@@ -6866,16 +6865,16 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>2</v>
@@ -6922,16 +6921,16 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>2</v>
@@ -6978,16 +6977,16 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>2</v>
@@ -7034,16 +7033,16 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>2</v>
@@ -7090,16 +7089,16 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>2</v>
@@ -7146,16 +7145,16 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>2</v>
@@ -7202,16 +7201,16 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>2</v>
@@ -7258,16 +7257,16 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>2</v>
@@ -7314,16 +7313,16 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>2</v>
@@ -7370,16 +7369,16 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>2</v>
@@ -7426,16 +7425,16 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>2</v>
@@ -7482,16 +7481,16 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>2</v>
@@ -7538,16 +7537,16 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>2</v>
@@ -7594,16 +7593,16 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>2</v>
@@ -7650,16 +7649,16 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>2</v>
@@ -7706,16 +7705,16 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>2</v>
@@ -7762,16 +7761,16 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>2</v>
@@ -7818,16 +7817,16 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>2</v>
@@ -7874,16 +7873,16 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>2</v>
@@ -7930,16 +7929,16 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>2</v>
@@ -7986,16 +7985,16 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>2</v>
@@ -8042,16 +8041,16 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>2</v>
@@ -8098,16 +8097,16 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>2</v>
@@ -8154,16 +8153,16 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E108" s="5" t="s">
         <v>2</v>
@@ -8210,16 +8209,16 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>2</v>
@@ -8266,16 +8265,16 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>2</v>
@@ -8322,16 +8321,16 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>2</v>
@@ -8378,16 +8377,16 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>2</v>
@@ -8434,16 +8433,16 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>2</v>
@@ -8490,16 +8489,16 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>2</v>
@@ -8546,16 +8545,16 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>2</v>
@@ -8602,16 +8601,16 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>2</v>
@@ -8658,16 +8657,16 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>2</v>
@@ -8714,16 +8713,16 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>2</v>
@@ -8770,16 +8769,16 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>2</v>
@@ -8826,16 +8825,16 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>2</v>
@@ -8882,16 +8881,16 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>2</v>
@@ -8938,16 +8937,16 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>2</v>
@@ -8994,16 +8993,16 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>2</v>
@@ -9462,7 +9461,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -9475,150 +9474,150 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B10" s="46" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B14" s="46" t="s">
         <v>23</v>
@@ -9629,35 +9628,35 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B15" s="49" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16" s="49" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made minor changes in 1. Helper = version based change (pickle library) 2. Added a snippet in the last function update_dam_routing_index to find the dam with the bas_id conflict. Still not resolved the issue. Dam GDW_ID: 38955
Additionally, changed the data type for a few columns (fields) of
dam and reservoir shapefile. Also, added GOID, INC, and BAS_ID fields in
the reservoir shapefile.

Updated the hydroRIVERS, and FFR shapefile, re-clipped again using the
new India shapefile.
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\GitHub\Free-Flowing-Rivers\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD9BAB-98F3-4100-9F9E-964A62CB7479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35579785-DF42-4904-998A-5C7827AC81CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="716" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,13 +671,13 @@
     <t>SED_try1</t>
   </si>
   <si>
-    <t>D:\RiverATLAS\Free_Flowing_Rivers\Mapping the worlds free-flowing rivers_Data_Geodatabase\Mapping the worlds free-flowing rivers_Data_Geodatabase\FFR_river_peninsular.gdb\FFR_river_peninsular</t>
-  </si>
-  <si>
     <t>CAP_MCM</t>
   </si>
   <si>
     <t>INCLUDE</t>
+  </si>
+  <si>
+    <t>D:\RiverATLAS\Free_Flowing_Rivers\FFR\FFR_peninsular_updated.shp</t>
   </si>
 </sst>
 </file>
@@ -1822,7 +1822,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1880,7 +1880,7 @@
         <v>Path to benchmark feature class</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>163</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>streams_fc</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D4" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1943,7 +1943,7 @@
         <v>barrier_inc_field</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D7" s="27" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2087,7 +2087,7 @@
         <v>svol_field</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" s="33" t="str">
         <f>Table8[[#This Row],[Short description]]</f>

</xml_diff>

<commit_message>
Set up for DOF and DOR. However, DOR values are not getting updated, says there is some GOID index error. DOF values are getting updated in the shapefile.
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\GitHub\Free-Flowing-Rivers\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35579785-DF42-4904-998A-5C7827AC81CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9EC3CF-3218-4425-B819-5105627418D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="716" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="33" r:id="rId1"/>
@@ -644,40 +644,40 @@
     <t>Field to use for storing SED values</t>
   </si>
   <si>
+    <t>C:\\FFR\data.gdb\bm_rivers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>D:\RiverATLAS\Global_Dam_Watch_GDW\GDW_filtered\GDW_reservoirs_filtered.shp</t>
+  </si>
+  <si>
+    <t>D:\RiverATLAS\Global_Dam_Watch_GDW\GDW_filtered\GDW_barriers_filtered.shp</t>
+  </si>
+  <si>
+    <t>D:\Peninsular India\Output</t>
+  </si>
+  <si>
+    <t>DOF_try1</t>
+  </si>
+  <si>
+    <t>DOR_try1</t>
+  </si>
+  <si>
+    <t>SED_try1</t>
+  </si>
+  <si>
+    <t>CAP_MCM</t>
+  </si>
+  <si>
+    <t>INCLUDE</t>
+  </si>
+  <si>
+    <t>D:\RiverATLAS\Free_Flowing_Rivers\FFR\FFR_peninsular_updated.shp</t>
+  </si>
+  <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>C:\\FFR\data.gdb\bm_rivers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>D:\RiverATLAS\Global_Dam_Watch_GDW\GDW_filtered\GDW_reservoirs_filtered.shp</t>
-  </si>
-  <si>
-    <t>D:\RiverATLAS\Global_Dam_Watch_GDW\GDW_filtered\GDW_barriers_filtered.shp</t>
-  </si>
-  <si>
-    <t>D:\Peninsular India\Output</t>
-  </si>
-  <si>
-    <t>DOF_try1</t>
-  </si>
-  <si>
-    <t>DOR_try1</t>
-  </si>
-  <si>
-    <t>SED_try1</t>
-  </si>
-  <si>
-    <t>CAP_MCM</t>
-  </si>
-  <si>
-    <t>INCLUDE</t>
-  </si>
-  <si>
-    <t>D:\RiverATLAS\Free_Flowing_Rivers\FFR\FFR_peninsular_updated.shp</t>
   </si>
 </sst>
 </file>
@@ -1733,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1783,7 @@
         <v>173</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>201</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1791,7 +1791,7 @@
         <v>174</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1799,7 +1799,7 @@
         <v>171</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1821,8 +1821,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1857,7 +1857,7 @@
         <v>dams_fc</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D2" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1873,7 +1873,7 @@
         <v>bench_fc</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1889,7 +1889,7 @@
         <v>streams_fc</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D4" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1905,7 +1905,7 @@
         <v>lakes_fc</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1927,7 +1927,7 @@
         <v>output_folder</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D6" s="23" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1943,7 +1943,7 @@
         <v>barrier_inc_field</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7" s="27" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -1991,7 +1991,7 @@
         <v>dof_field</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D10" s="30" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2071,7 +2071,7 @@
         <v>dor_field</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D15" s="33" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2087,7 +2087,7 @@
         <v>svol_field</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16" s="33" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2109,7 +2109,7 @@
         <v>sed_field</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D17" s="36" t="str">
         <f>Table8[[#This Row],[Short description]]</f>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
@@ -9461,7 +9461,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>